<commit_message>
Typo corrected in sheet 2 title
</commit_message>
<xml_diff>
--- a/Data/Diarrhoea_Treatments_Mongu.xlsx
+++ b/Data/Diarrhoea_Treatments_Mongu.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Durham\Desktop\Academia\Other Projects\Statisticians4Society\Data\Version_for_Repository\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Durham\Desktop\Academia\Other Projects\Statisticians4Society\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9373BE-1BF1-4C71-9E95-17984D475E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F508C644-42C3-4B75-AE97-61714BB2EFC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="23040" windowHeight="11640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="62">
   <si>
     <t># of cases given another treatment</t>
   </si>
@@ -420,6 +420,9 @@
   </si>
   <si>
     <t>health_facility</t>
+  </si>
+  <si>
+    <t>Data October 2016 (records from tally sheets)</t>
   </si>
 </sst>
 </file>
@@ -1693,7 +1696,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="34" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="24" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>